<commit_message>
shortest path all nodes and edges  and draw them
</commit_message>
<xml_diff>
--- a/notebooks/edges.xlsx
+++ b/notebooks/edges.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J393"/>
+  <dimension ref="A1:I393"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,11 +479,6 @@
           <t>time</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>weights</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -517,9 +512,6 @@
       <c r="I2" t="n">
         <v>0.04291888590753235</v>
       </c>
-      <c r="J2" t="n">
-        <v>858</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -553,9 +545,6 @@
       <c r="I3" t="n">
         <v>0.01189814320740397</v>
       </c>
-      <c r="J3" t="n">
-        <v>237</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -589,9 +578,6 @@
       <c r="I4" t="n">
         <v>0.06600495287173748</v>
       </c>
-      <c r="J4" t="n">
-        <v>1320</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -625,9 +611,6 @@
       <c r="I5" t="n">
         <v>0.04513773078850408</v>
       </c>
-      <c r="J5" t="n">
-        <v>902</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -661,9 +644,6 @@
       <c r="I6" t="n">
         <v>0.04254828604533498</v>
       </c>
-      <c r="J6" t="n">
-        <v>850</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -697,9 +677,6 @@
       <c r="I7" t="n">
         <v>0.05750973685698733</v>
       </c>
-      <c r="J7" t="n">
-        <v>1150</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -733,9 +710,6 @@
       <c r="I8" t="n">
         <v>0.08093604043326326</v>
       </c>
-      <c r="J8" t="n">
-        <v>1618</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -769,9 +743,6 @@
       <c r="I9" t="n">
         <v>0.1092645753752804</v>
       </c>
-      <c r="J9" t="n">
-        <v>2185</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -805,9 +776,6 @@
       <c r="I10" t="n">
         <v>0.002301435776846543</v>
       </c>
-      <c r="J10" t="n">
-        <v>46</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -841,9 +809,6 @@
       <c r="I11" t="n">
         <v>0.0218445915482741</v>
       </c>
-      <c r="J11" t="n">
-        <v>436</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -877,9 +842,6 @@
       <c r="I12" t="n">
         <v>0.03187661257935191</v>
       </c>
-      <c r="J12" t="n">
-        <v>637</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -913,9 +875,6 @@
       <c r="I13" t="n">
         <v>0.08333207680680628</v>
       </c>
-      <c r="J13" t="n">
-        <v>1666</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -949,9 +908,6 @@
       <c r="I14" t="n">
         <v>0.052587060091626</v>
       </c>
-      <c r="J14" t="n">
-        <v>1051</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -985,9 +941,6 @@
       <c r="I15" t="n">
         <v>0.002119198473795245</v>
       </c>
-      <c r="J15" t="n">
-        <v>42</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1021,9 +974,6 @@
       <c r="I16" t="n">
         <v>0.02009110806847891</v>
       </c>
-      <c r="J16" t="n">
-        <v>401</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1061,9 +1011,6 @@
       <c r="I17" t="n">
         <v>0.01007479228801522</v>
       </c>
-      <c r="J17" t="n">
-        <v>201</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1101,9 +1048,6 @@
       <c r="I18" t="n">
         <v>0.001154445024260076</v>
       </c>
-      <c r="J18" t="n">
-        <v>23</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1141,9 +1085,6 @@
       <c r="I19" t="n">
         <v>0.001118125627446256</v>
       </c>
-      <c r="J19" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1181,9 +1122,6 @@
       <c r="I20" t="n">
         <v>0.006905458988114566</v>
       </c>
-      <c r="J20" t="n">
-        <v>138</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1221,9 +1159,6 @@
       <c r="I21" t="n">
         <v>0.003283900143112685</v>
       </c>
-      <c r="J21" t="n">
-        <v>65</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1261,9 +1196,6 @@
       <c r="I22" t="n">
         <v>0.001124684235573434</v>
       </c>
-      <c r="J22" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1301,9 +1233,6 @@
       <c r="I23" t="n">
         <v>0.009957243440214975</v>
       </c>
-      <c r="J23" t="n">
-        <v>199</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1341,9 +1270,6 @@
       <c r="I24" t="n">
         <v>0.002920080221141457</v>
       </c>
-      <c r="J24" t="n">
-        <v>58</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1381,9 +1307,6 @@
       <c r="I25" t="n">
         <v>0.001453814738740543</v>
       </c>
-      <c r="J25" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1421,9 +1344,6 @@
       <c r="I26" t="n">
         <v>0.001034743054666413</v>
       </c>
-      <c r="J26" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1461,9 +1381,6 @@
       <c r="I27" t="n">
         <v>0.00270449852200725</v>
       </c>
-      <c r="J27" t="n">
-        <v>54</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1501,9 +1418,6 @@
       <c r="I28" t="n">
         <v>0.01593082689651963</v>
       </c>
-      <c r="J28" t="n">
-        <v>318</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1541,9 +1455,6 @@
       <c r="I29" t="n">
         <v>0.005412021336487831</v>
       </c>
-      <c r="J29" t="n">
-        <v>108</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1581,9 +1492,6 @@
       <c r="I30" t="n">
         <v>0.008003619583382878</v>
       </c>
-      <c r="J30" t="n">
-        <v>160</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1621,9 +1529,6 @@
       <c r="I31" t="n">
         <v>0.01443702003548247</v>
       </c>
-      <c r="J31" t="n">
-        <v>288</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1660,9 +1565,6 @@
       </c>
       <c r="I32" t="n">
         <v>0.001238754559963717</v>
-      </c>
-      <c r="J32" t="n">
-        <v>24</v>
       </c>
     </row>
     <row r="33">
@@ -1697,9 +1599,6 @@
       <c r="I33" t="n">
         <v>0.02947843192703213</v>
       </c>
-      <c r="J33" t="n">
-        <v>589</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1733,9 +1632,6 @@
       <c r="I34" t="n">
         <v>0.01913865238364538</v>
       </c>
-      <c r="J34" t="n">
-        <v>382</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1769,9 +1665,6 @@
       <c r="I35" t="n">
         <v>0.03151362427051979</v>
       </c>
-      <c r="J35" t="n">
-        <v>630</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1805,9 +1698,6 @@
       <c r="I36" t="n">
         <v>0.1056249492787319</v>
       </c>
-      <c r="J36" t="n">
-        <v>2112</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1845,9 +1735,6 @@
       <c r="I37" t="n">
         <v>0.002990876058229087</v>
       </c>
-      <c r="J37" t="n">
-        <v>59</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1885,9 +1772,6 @@
       <c r="I38" t="n">
         <v>0.001896612867711132</v>
       </c>
-      <c r="J38" t="n">
-        <v>37</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1925,9 +1809,6 @@
       <c r="I39" t="n">
         <v>0.02533264211764506</v>
       </c>
-      <c r="J39" t="n">
-        <v>506</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1965,9 +1846,6 @@
       <c r="I40" t="n">
         <v>0.00288633480951035</v>
       </c>
-      <c r="J40" t="n">
-        <v>57</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2005,9 +1883,6 @@
       <c r="I41" t="n">
         <v>0.02302512425716172</v>
       </c>
-      <c r="J41" t="n">
-        <v>460</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2045,9 +1920,6 @@
       <c r="I42" t="n">
         <v>0.0009171508856151261</v>
       </c>
-      <c r="J42" t="n">
-        <v>18</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2084,9 +1956,6 @@
       </c>
       <c r="I43" t="n">
         <v>0.00267388230873784</v>
-      </c>
-      <c r="J43" t="n">
-        <v>53</v>
       </c>
     </row>
     <row r="44">
@@ -2121,9 +1990,6 @@
       <c r="I44" t="n">
         <v>0.005551892558349555</v>
       </c>
-      <c r="J44" t="n">
-        <v>111</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2157,9 +2023,6 @@
       <c r="I45" t="n">
         <v>0.0003799366924722342</v>
       </c>
-      <c r="J45" t="n">
-        <v>7</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2193,9 +2056,6 @@
       <c r="I46" t="n">
         <v>0.01628820502718714</v>
       </c>
-      <c r="J46" t="n">
-        <v>325</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2229,9 +2089,6 @@
       <c r="I47" t="n">
         <v>0.0161664711396996</v>
       </c>
-      <c r="J47" t="n">
-        <v>323</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2265,9 +2122,6 @@
       <c r="I48" t="n">
         <v>0.06010780199156748</v>
       </c>
-      <c r="J48" t="n">
-        <v>1202</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2301,9 +2155,6 @@
       <c r="I49" t="n">
         <v>0.0829864216058542</v>
       </c>
-      <c r="J49" t="n">
-        <v>1659</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2337,9 +2188,6 @@
       <c r="I50" t="n">
         <v>0.0006942597199702168</v>
       </c>
-      <c r="J50" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2373,9 +2221,6 @@
       <c r="I51" t="n">
         <v>0.002958217622912613</v>
       </c>
-      <c r="J51" t="n">
-        <v>59</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2413,9 +2258,6 @@
       <c r="I52" t="n">
         <v>0.007858482236407048</v>
       </c>
-      <c r="J52" t="n">
-        <v>157</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2453,9 +2295,6 @@
       <c r="I53" t="n">
         <v>0.001149715668440909</v>
       </c>
-      <c r="J53" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2492,9 +2331,6 @@
       </c>
       <c r="I54" t="n">
         <v>0.009890861861751622</v>
-      </c>
-      <c r="J54" t="n">
-        <v>197</v>
       </c>
     </row>
     <row r="55">
@@ -2529,9 +2365,6 @@
       <c r="I55" t="n">
         <v>0.03579764862525003</v>
       </c>
-      <c r="J55" t="n">
-        <v>715</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2565,9 +2398,6 @@
       <c r="I56" t="n">
         <v>0.08863477734276196</v>
       </c>
-      <c r="J56" t="n">
-        <v>1772</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2601,9 +2431,6 @@
       <c r="I57" t="n">
         <v>0.01612458415440934</v>
       </c>
-      <c r="J57" t="n">
-        <v>322</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2637,9 +2464,6 @@
       <c r="I58" t="n">
         <v>0.0006704041283828914</v>
       </c>
-      <c r="J58" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2673,9 +2497,6 @@
       <c r="I59" t="n">
         <v>0.07075983945829079</v>
       </c>
-      <c r="J59" t="n">
-        <v>1415</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2709,9 +2530,6 @@
       <c r="I60" t="n">
         <v>0.00231230712384655</v>
       </c>
-      <c r="J60" t="n">
-        <v>46</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2745,9 +2563,6 @@
       <c r="I61" t="n">
         <v>0.002957206571049549</v>
       </c>
-      <c r="J61" t="n">
-        <v>59</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2781,9 +2596,6 @@
       <c r="I62" t="n">
         <v>0.06812741960019064</v>
       </c>
-      <c r="J62" t="n">
-        <v>1362</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2817,9 +2629,6 @@
       <c r="I63" t="n">
         <v>0.002295724900405671</v>
       </c>
-      <c r="J63" t="n">
-        <v>45</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2857,9 +2666,6 @@
       <c r="I64" t="n">
         <v>0.009830303427269718</v>
       </c>
-      <c r="J64" t="n">
-        <v>196</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2897,9 +2703,6 @@
       <c r="I65" t="n">
         <v>0.009891344734754705</v>
       </c>
-      <c r="J65" t="n">
-        <v>197</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2937,9 +2740,6 @@
       <c r="I66" t="n">
         <v>0.003385059581417977</v>
       </c>
-      <c r="J66" t="n">
-        <v>67</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2977,9 +2777,6 @@
       <c r="I67" t="n">
         <v>0.003508952651956756</v>
       </c>
-      <c r="J67" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3017,9 +2814,6 @@
       <c r="I68" t="n">
         <v>0.00438849731015941</v>
       </c>
-      <c r="J68" t="n">
-        <v>87</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3057,9 +2851,6 @@
       <c r="I69" t="n">
         <v>0.02064522247344264</v>
       </c>
-      <c r="J69" t="n">
-        <v>412</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3097,9 +2888,6 @@
       <c r="I70" t="n">
         <v>0.001936795509300123</v>
       </c>
-      <c r="J70" t="n">
-        <v>38</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3137,9 +2925,6 @@
       <c r="I71" t="n">
         <v>0.01777901156412939</v>
       </c>
-      <c r="J71" t="n">
-        <v>355</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3177,9 +2962,6 @@
       <c r="I72" t="n">
         <v>0.004401868074606251</v>
       </c>
-      <c r="J72" t="n">
-        <v>88</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3216,9 +2998,6 @@
       </c>
       <c r="I73" t="n">
         <v>0.004517583463994706</v>
-      </c>
-      <c r="J73" t="n">
-        <v>90</v>
       </c>
     </row>
     <row r="74">
@@ -3253,9 +3032,6 @@
       <c r="I74" t="n">
         <v>0.01547116466785542</v>
       </c>
-      <c r="J74" t="n">
-        <v>309</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3293,9 +3069,6 @@
       <c r="I75" t="n">
         <v>0.002308285263593414</v>
       </c>
-      <c r="J75" t="n">
-        <v>46</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3332,9 +3105,6 @@
       </c>
       <c r="I76" t="n">
         <v>0.002306403743778633</v>
-      </c>
-      <c r="J76" t="n">
-        <v>46</v>
       </c>
     </row>
     <row r="77">
@@ -3369,9 +3139,6 @@
       <c r="I77" t="n">
         <v>0.05637609161533424</v>
       </c>
-      <c r="J77" t="n">
-        <v>1127</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3409,9 +3176,6 @@
       <c r="I78" t="n">
         <v>0.006222347980911108</v>
       </c>
-      <c r="J78" t="n">
-        <v>124</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3449,9 +3213,6 @@
       <c r="I79" t="n">
         <v>0.0121687110887214</v>
       </c>
-      <c r="J79" t="n">
-        <v>243</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3489,9 +3250,6 @@
       <c r="I80" t="n">
         <v>0.006742706732389658</v>
       </c>
-      <c r="J80" t="n">
-        <v>134</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3528,9 +3286,6 @@
       </c>
       <c r="I81" t="n">
         <v>0.01674035901402205</v>
-      </c>
-      <c r="J81" t="n">
-        <v>334</v>
       </c>
     </row>
     <row r="82">
@@ -3565,9 +3320,6 @@
       <c r="I82" t="n">
         <v>0.02306311805488968</v>
       </c>
-      <c r="J82" t="n">
-        <v>461</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3601,9 +3353,6 @@
       <c r="I83" t="n">
         <v>0.001239894862743176</v>
       </c>
-      <c r="J83" t="n">
-        <v>24</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3641,9 +3390,6 @@
       <c r="I84" t="n">
         <v>0.000300525371424899</v>
       </c>
-      <c r="J84" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3681,9 +3427,6 @@
       <c r="I85" t="n">
         <v>0.007725687472272668</v>
       </c>
-      <c r="J85" t="n">
-        <v>154</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3721,9 +3464,6 @@
       <c r="I86" t="n">
         <v>0.002415152074583929</v>
       </c>
-      <c r="J86" t="n">
-        <v>48</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3761,9 +3501,6 @@
       <c r="I87" t="n">
         <v>0.0009978543783647766</v>
       </c>
-      <c r="J87" t="n">
-        <v>19</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3800,9 +3537,6 @@
       </c>
       <c r="I88" t="n">
         <v>0.01830168897903272</v>
-      </c>
-      <c r="J88" t="n">
-        <v>366</v>
       </c>
     </row>
     <row r="89">
@@ -3837,9 +3571,6 @@
       <c r="I89" t="n">
         <v>0.05306663573069251</v>
       </c>
-      <c r="J89" t="n">
-        <v>1061</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3876,9 +3607,6 @@
       </c>
       <c r="I90" t="n">
         <v>0.006424896216529034</v>
-      </c>
-      <c r="J90" t="n">
-        <v>128</v>
       </c>
     </row>
     <row r="91">
@@ -3913,9 +3641,6 @@
       <c r="I91" t="n">
         <v>0.03433742580187332</v>
       </c>
-      <c r="J91" t="n">
-        <v>686</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3949,9 +3674,6 @@
       <c r="I92" t="n">
         <v>0.05020470890161086</v>
       </c>
-      <c r="J92" t="n">
-        <v>1004</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3985,9 +3707,6 @@
       <c r="I93" t="n">
         <v>0.001181941592191626</v>
       </c>
-      <c r="J93" t="n">
-        <v>23</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4024,9 +3743,6 @@
       </c>
       <c r="I94" t="n">
         <v>0.007030912713266139</v>
-      </c>
-      <c r="J94" t="n">
-        <v>140</v>
       </c>
     </row>
     <row r="95">
@@ -4061,9 +3777,6 @@
       <c r="I95" t="n">
         <v>0.001886909328008667</v>
       </c>
-      <c r="J95" t="n">
-        <v>37</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4097,9 +3810,6 @@
       <c r="I96" t="n">
         <v>0.01101290753662803</v>
       </c>
-      <c r="J96" t="n">
-        <v>220</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4133,9 +3843,6 @@
       <c r="I97" t="n">
         <v>0.01353580763728603</v>
       </c>
-      <c r="J97" t="n">
-        <v>270</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4169,9 +3876,6 @@
       <c r="I98" t="n">
         <v>0.009889566969877493</v>
       </c>
-      <c r="J98" t="n">
-        <v>197</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4205,9 +3909,6 @@
       <c r="I99" t="n">
         <v>0.01469093905618701</v>
       </c>
-      <c r="J99" t="n">
-        <v>293</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4241,9 +3942,6 @@
       <c r="I100" t="n">
         <v>0.07942153902260882</v>
       </c>
-      <c r="J100" t="n">
-        <v>1588</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4277,9 +3975,6 @@
       <c r="I101" t="n">
         <v>0.006724351682965466</v>
       </c>
-      <c r="J101" t="n">
-        <v>134</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4313,9 +4008,6 @@
       <c r="I102" t="n">
         <v>0.08361508507705409</v>
       </c>
-      <c r="J102" t="n">
-        <v>1672</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4349,9 +4041,6 @@
       <c r="I103" t="n">
         <v>0.0006793560541118616</v>
       </c>
-      <c r="J103" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4385,9 +4074,6 @@
       <c r="I104" t="n">
         <v>0.001875677464346382</v>
       </c>
-      <c r="J104" t="n">
-        <v>37</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4421,9 +4107,6 @@
       <c r="I105" t="n">
         <v>0.01103188808006804</v>
       </c>
-      <c r="J105" t="n">
-        <v>220</v>
-      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4461,9 +4144,6 @@
       <c r="I106" t="n">
         <v>0.00678151674026548</v>
       </c>
-      <c r="J106" t="n">
-        <v>135</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4500,9 +4180,6 @@
       </c>
       <c r="I107" t="n">
         <v>0.006879091758084205</v>
-      </c>
-      <c r="J107" t="n">
-        <v>137</v>
       </c>
     </row>
     <row r="108">
@@ -4537,9 +4214,6 @@
       <c r="I108" t="n">
         <v>0.006847568112009089</v>
       </c>
-      <c r="J108" t="n">
-        <v>136</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4573,9 +4247,6 @@
       <c r="I109" t="n">
         <v>0.007020347681892299</v>
       </c>
-      <c r="J109" t="n">
-        <v>140</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4609,9 +4280,6 @@
       <c r="I110" t="n">
         <v>0.05842729669191598</v>
       </c>
-      <c r="J110" t="n">
-        <v>1168</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4648,9 +4316,6 @@
       </c>
       <c r="I111" t="n">
         <v>0.009901886502176783</v>
-      </c>
-      <c r="J111" t="n">
-        <v>198</v>
       </c>
     </row>
     <row r="112">
@@ -4685,9 +4350,6 @@
       <c r="I112" t="n">
         <v>0.004703586783554438</v>
       </c>
-      <c r="J112" t="n">
-        <v>94</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4721,9 +4383,6 @@
       <c r="I113" t="n">
         <v>0.005617183875649012</v>
       </c>
-      <c r="J113" t="n">
-        <v>112</v>
-      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4757,9 +4416,6 @@
       <c r="I114" t="n">
         <v>0.005962987560648659</v>
       </c>
-      <c r="J114" t="n">
-        <v>119</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4793,9 +4449,6 @@
       <c r="I115" t="n">
         <v>0.004532921479339807</v>
       </c>
-      <c r="J115" t="n">
-        <v>90</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4829,9 +4482,6 @@
       <c r="I116" t="n">
         <v>0.006652086854670678</v>
       </c>
-      <c r="J116" t="n">
-        <v>133</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4865,9 +4515,6 @@
       <c r="I117" t="n">
         <v>0.03012795871165942</v>
       </c>
-      <c r="J117" t="n">
-        <v>602</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4901,9 +4548,6 @@
       <c r="I118" t="n">
         <v>0.001523526096969922</v>
       </c>
-      <c r="J118" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -4937,9 +4581,6 @@
       <c r="I119" t="n">
         <v>0.001497340573217734</v>
       </c>
-      <c r="J119" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4977,9 +4618,6 @@
       <c r="I120" t="n">
         <v>0.02293380207437021</v>
       </c>
-      <c r="J120" t="n">
-        <v>458</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -5016,9 +4654,6 @@
       </c>
       <c r="I121" t="n">
         <v>0.002333627929493452</v>
-      </c>
-      <c r="J121" t="n">
-        <v>46</v>
       </c>
     </row>
     <row r="122">
@@ -5053,9 +4688,6 @@
       <c r="I122" t="n">
         <v>0.03517057003962695</v>
       </c>
-      <c r="J122" t="n">
-        <v>703</v>
-      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5089,9 +4721,6 @@
       <c r="I123" t="n">
         <v>0.01909981552520178</v>
       </c>
-      <c r="J123" t="n">
-        <v>381</v>
-      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5125,9 +4754,6 @@
       <c r="I124" t="n">
         <v>0.03570719570302837</v>
       </c>
-      <c r="J124" t="n">
-        <v>714</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5161,9 +4787,6 @@
       <c r="I125" t="n">
         <v>0.01796575365172033</v>
       </c>
-      <c r="J125" t="n">
-        <v>359</v>
-      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5201,9 +4824,6 @@
       <c r="I126" t="n">
         <v>0.00328572465264281</v>
       </c>
-      <c r="J126" t="n">
-        <v>65</v>
-      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5241,9 +4861,6 @@
       <c r="I127" t="n">
         <v>0.004217108060053162</v>
       </c>
-      <c r="J127" t="n">
-        <v>84</v>
-      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5281,9 +4898,6 @@
       <c r="I128" t="n">
         <v>0.001521654071846883</v>
       </c>
-      <c r="J128" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -5320,9 +4934,6 @@
       </c>
       <c r="I129" t="n">
         <v>0.004028938426753335</v>
-      </c>
-      <c r="J129" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="130">
@@ -5357,9 +4968,6 @@
       <c r="I130" t="n">
         <v>0.01537479532751783</v>
       </c>
-      <c r="J130" t="n">
-        <v>307</v>
-      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -5393,9 +5001,6 @@
       <c r="I131" t="n">
         <v>0.00663489873103423</v>
       </c>
-      <c r="J131" t="n">
-        <v>132</v>
-      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -5433,9 +5038,6 @@
       <c r="I132" t="n">
         <v>0.004014404538893163</v>
       </c>
-      <c r="J132" t="n">
-        <v>80</v>
-      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -5472,9 +5074,6 @@
       </c>
       <c r="I133" t="n">
         <v>0.02439303470037178</v>
-      </c>
-      <c r="J133" t="n">
-        <v>487</v>
       </c>
     </row>
     <row r="134">
@@ -5509,9 +5108,6 @@
       <c r="I134" t="n">
         <v>0.1010780449072587</v>
       </c>
-      <c r="J134" t="n">
-        <v>2021</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5545,9 +5141,6 @@
       <c r="I135" t="n">
         <v>0.01233934717784403</v>
       </c>
-      <c r="J135" t="n">
-        <v>246</v>
-      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -5581,9 +5174,6 @@
       <c r="I136" t="n">
         <v>0.02879021004622008</v>
       </c>
-      <c r="J136" t="n">
-        <v>575</v>
-      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -5617,9 +5207,6 @@
       <c r="I137" t="n">
         <v>0.08135431307784943</v>
       </c>
-      <c r="J137" t="n">
-        <v>1627</v>
-      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5657,9 +5244,6 @@
       <c r="I138" t="n">
         <v>0.008561675627532569</v>
       </c>
-      <c r="J138" t="n">
-        <v>171</v>
-      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5697,9 +5281,6 @@
       <c r="I139" t="n">
         <v>0.008559278966216244</v>
       </c>
-      <c r="J139" t="n">
-        <v>171</v>
-      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5736,9 +5317,6 @@
       </c>
       <c r="I140" t="n">
         <v>0.001500149094537392</v>
-      </c>
-      <c r="J140" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="141">
@@ -5773,9 +5351,6 @@
       <c r="I141" t="n">
         <v>0.002294769085421859</v>
       </c>
-      <c r="J141" t="n">
-        <v>45</v>
-      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -5809,9 +5384,6 @@
       <c r="I142" t="n">
         <v>0.07905755349454242</v>
       </c>
-      <c r="J142" t="n">
-        <v>1581</v>
-      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -5849,9 +5421,6 @@
       <c r="I143" t="n">
         <v>0.01125981916214867</v>
       </c>
-      <c r="J143" t="n">
-        <v>225</v>
-      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -5888,9 +5457,6 @@
       </c>
       <c r="I144" t="n">
         <v>0.01211729484279254</v>
-      </c>
-      <c r="J144" t="n">
-        <v>242</v>
       </c>
     </row>
     <row r="145">
@@ -5925,9 +5491,6 @@
       <c r="I145" t="n">
         <v>0.01098621032348964</v>
       </c>
-      <c r="J145" t="n">
-        <v>219</v>
-      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -5961,9 +5524,6 @@
       <c r="I146" t="n">
         <v>0.004986323096546279</v>
       </c>
-      <c r="J146" t="n">
-        <v>99</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -6000,9 +5560,6 @@
       </c>
       <c r="I147" t="n">
         <v>0.01876789114047425</v>
-      </c>
-      <c r="J147" t="n">
-        <v>375</v>
       </c>
     </row>
     <row r="148">
@@ -6037,9 +5594,6 @@
       <c r="I148" t="n">
         <v>0.002598281501902311</v>
       </c>
-      <c r="J148" t="n">
-        <v>51</v>
-      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -6073,9 +5627,6 @@
       <c r="I149" t="n">
         <v>0.09875062754310852</v>
       </c>
-      <c r="J149" t="n">
-        <v>1975</v>
-      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -6109,9 +5660,6 @@
       <c r="I150" t="n">
         <v>0.02704107666809312</v>
       </c>
-      <c r="J150" t="n">
-        <v>540</v>
-      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -6145,9 +5693,6 @@
       <c r="I151" t="n">
         <v>0.01097808960115464</v>
       </c>
-      <c r="J151" t="n">
-        <v>219</v>
-      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -6181,9 +5726,6 @@
       <c r="I152" t="n">
         <v>0.002883516922546546</v>
       </c>
-      <c r="J152" t="n">
-        <v>57</v>
-      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -6217,9 +5759,6 @@
       <c r="I153" t="n">
         <v>0.09290229842233552</v>
       </c>
-      <c r="J153" t="n">
-        <v>1858</v>
-      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -6253,9 +5792,6 @@
       <c r="I154" t="n">
         <v>0.002893451690112056</v>
       </c>
-      <c r="J154" t="n">
-        <v>57</v>
-      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -6289,9 +5825,6 @@
       <c r="I155" t="n">
         <v>0.03234876689075921</v>
       </c>
-      <c r="J155" t="n">
-        <v>646</v>
-      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -6325,9 +5858,6 @@
       <c r="I156" t="n">
         <v>0.05414129212446556</v>
       </c>
-      <c r="J156" t="n">
-        <v>1082</v>
-      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -6364,9 +5894,6 @@
       </c>
       <c r="I157" t="n">
         <v>0.01481821703579644</v>
-      </c>
-      <c r="J157" t="n">
-        <v>296</v>
       </c>
     </row>
     <row r="158">
@@ -6401,9 +5928,6 @@
       <c r="I158" t="n">
         <v>0.002163583091953283</v>
       </c>
-      <c r="J158" t="n">
-        <v>43</v>
-      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -6440,9 +5964,6 @@
       </c>
       <c r="I159" t="n">
         <v>0.01830219846906479</v>
-      </c>
-      <c r="J159" t="n">
-        <v>366</v>
       </c>
     </row>
     <row r="160">
@@ -6477,9 +5998,6 @@
       <c r="I160" t="n">
         <v>0.08380375201138385</v>
       </c>
-      <c r="J160" t="n">
-        <v>1676</v>
-      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -6513,9 +6031,6 @@
       <c r="I161" t="n">
         <v>0.005219721280331401</v>
       </c>
-      <c r="J161" t="n">
-        <v>104</v>
-      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -6553,9 +6068,6 @@
       <c r="I162" t="n">
         <v>0.02119179683513352</v>
       </c>
-      <c r="J162" t="n">
-        <v>423</v>
-      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -6593,9 +6105,6 @@
       <c r="I163" t="n">
         <v>0.01121815277333651</v>
       </c>
-      <c r="J163" t="n">
-        <v>224</v>
-      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -6633,9 +6142,6 @@
       <c r="I164" t="n">
         <v>0.01595978278279839</v>
       </c>
-      <c r="J164" t="n">
-        <v>319</v>
-      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -6673,9 +6179,6 @@
       <c r="I165" t="n">
         <v>0.0009704268224800035</v>
       </c>
-      <c r="J165" t="n">
-        <v>19</v>
-      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -6713,9 +6216,6 @@
       <c r="I166" t="n">
         <v>0.0009881672211748858</v>
       </c>
-      <c r="J166" t="n">
-        <v>19</v>
-      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -6753,9 +6253,6 @@
       <c r="I167" t="n">
         <v>0.00146827564561986</v>
       </c>
-      <c r="J167" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -6792,9 +6289,6 @@
       </c>
       <c r="I168" t="n">
         <v>0.001637884628167427</v>
-      </c>
-      <c r="J168" t="n">
-        <v>32</v>
       </c>
     </row>
     <row r="169">
@@ -6829,9 +6323,6 @@
       <c r="I169" t="n">
         <v>0.00839499195029997</v>
       </c>
-      <c r="J169" t="n">
-        <v>167</v>
-      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -6865,9 +6356,6 @@
       <c r="I170" t="n">
         <v>0.04952556108644326</v>
       </c>
-      <c r="J170" t="n">
-        <v>990</v>
-      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -6905,9 +6393,6 @@
       <c r="I171" t="n">
         <v>0.01405158353452475</v>
       </c>
-      <c r="J171" t="n">
-        <v>281</v>
-      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -6945,9 +6430,6 @@
       <c r="I172" t="n">
         <v>0.01286061874358826</v>
       </c>
-      <c r="J172" t="n">
-        <v>257</v>
-      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -6985,9 +6467,6 @@
       <c r="I173" t="n">
         <v>0.01380541549170093</v>
       </c>
-      <c r="J173" t="n">
-        <v>276</v>
-      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -7024,9 +6503,6 @@
       </c>
       <c r="I174" t="n">
         <v>0.01285437785015225</v>
-      </c>
-      <c r="J174" t="n">
-        <v>257</v>
       </c>
     </row>
     <row r="175">
@@ -7061,9 +6537,6 @@
       <c r="I175" t="n">
         <v>0.005267517739846117</v>
       </c>
-      <c r="J175" t="n">
-        <v>105</v>
-      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -7101,9 +6574,6 @@
       <c r="I176" t="n">
         <v>0.005532591915833859</v>
       </c>
-      <c r="J176" t="n">
-        <v>110</v>
-      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -7141,9 +6611,6 @@
       <c r="I177" t="n">
         <v>0.01106938231379094</v>
       </c>
-      <c r="J177" t="n">
-        <v>221</v>
-      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -7181,9 +6648,6 @@
       <c r="I178" t="n">
         <v>0.001510372548055439</v>
       </c>
-      <c r="J178" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -7221,9 +6685,6 @@
       <c r="I179" t="n">
         <v>0.001131364005438877</v>
       </c>
-      <c r="J179" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -7261,9 +6722,6 @@
       <c r="I180" t="n">
         <v>0.004752390698448142</v>
       </c>
-      <c r="J180" t="n">
-        <v>95</v>
-      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -7301,9 +6759,6 @@
       <c r="I181" t="n">
         <v>0.01162228776233277</v>
       </c>
-      <c r="J181" t="n">
-        <v>232</v>
-      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -7341,9 +6796,6 @@
       <c r="I182" t="n">
         <v>0.002383295889097159</v>
       </c>
-      <c r="J182" t="n">
-        <v>47</v>
-      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -7381,9 +6833,6 @@
       <c r="I183" t="n">
         <v>0.002528055041439558</v>
       </c>
-      <c r="J183" t="n">
-        <v>50</v>
-      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -7421,9 +6870,6 @@
       <c r="I184" t="n">
         <v>0.002539935906796013</v>
       </c>
-      <c r="J184" t="n">
-        <v>50</v>
-      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -7461,9 +6907,6 @@
       <c r="I185" t="n">
         <v>0.001084614409600265</v>
       </c>
-      <c r="J185" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -7501,9 +6944,6 @@
       <c r="I186" t="n">
         <v>0.003860303278707322</v>
       </c>
-      <c r="J186" t="n">
-        <v>77</v>
-      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -7541,9 +6981,6 @@
       <c r="I187" t="n">
         <v>0.003840814185652634</v>
       </c>
-      <c r="J187" t="n">
-        <v>76</v>
-      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -7581,9 +7018,6 @@
       <c r="I188" t="n">
         <v>0.003316428322647356</v>
       </c>
-      <c r="J188" t="n">
-        <v>66</v>
-      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -7620,9 +7054,6 @@
       </c>
       <c r="I189" t="n">
         <v>0.002056309260441618</v>
-      </c>
-      <c r="J189" t="n">
-        <v>41</v>
       </c>
     </row>
     <row r="190">
@@ -7657,9 +7088,6 @@
       <c r="I190" t="n">
         <v>0.005651159603041828</v>
       </c>
-      <c r="J190" t="n">
-        <v>113</v>
-      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -7693,9 +7121,6 @@
       <c r="I191" t="n">
         <v>0.01480748305045563</v>
       </c>
-      <c r="J191" t="n">
-        <v>296</v>
-      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -7729,9 +7154,6 @@
       <c r="I192" t="n">
         <v>0.004149385189596962</v>
       </c>
-      <c r="J192" t="n">
-        <v>82</v>
-      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -7765,9 +7187,6 @@
       <c r="I193" t="n">
         <v>0.0691227229942375</v>
       </c>
-      <c r="J193" t="n">
-        <v>1382</v>
-      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -7801,9 +7220,6 @@
       <c r="I194" t="n">
         <v>0.009255062988768322</v>
       </c>
-      <c r="J194" t="n">
-        <v>185</v>
-      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -7837,9 +7253,6 @@
       <c r="I195" t="n">
         <v>0.02444989859986035</v>
       </c>
-      <c r="J195" t="n">
-        <v>488</v>
-      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -7877,9 +7290,6 @@
       <c r="I196" t="n">
         <v>0.002902037985890595</v>
       </c>
-      <c r="J196" t="n">
-        <v>58</v>
-      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -7917,9 +7327,6 @@
       <c r="I197" t="n">
         <v>0.00249306665618009</v>
       </c>
-      <c r="J197" t="n">
-        <v>49</v>
-      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -7957,9 +7364,6 @@
       <c r="I198" t="n">
         <v>0.005985132349789031</v>
       </c>
-      <c r="J198" t="n">
-        <v>119</v>
-      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -7997,9 +7401,6 @@
       <c r="I199" t="n">
         <v>0.01137701257388542</v>
       </c>
-      <c r="J199" t="n">
-        <v>227</v>
-      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -8037,9 +7438,6 @@
       <c r="I200" t="n">
         <v>0.01302729815954464</v>
       </c>
-      <c r="J200" t="n">
-        <v>260</v>
-      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -8077,9 +7475,6 @@
       <c r="I201" t="n">
         <v>0.01414189077071227</v>
       </c>
-      <c r="J201" t="n">
-        <v>282</v>
-      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -8117,9 +7512,6 @@
       <c r="I202" t="n">
         <v>0.002319494257089317</v>
       </c>
-      <c r="J202" t="n">
-        <v>46</v>
-      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -8157,9 +7549,6 @@
       <c r="I203" t="n">
         <v>0.008972005842293108</v>
       </c>
-      <c r="J203" t="n">
-        <v>179</v>
-      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -8197,9 +7586,6 @@
       <c r="I204" t="n">
         <v>0.001156627362465251</v>
       </c>
-      <c r="J204" t="n">
-        <v>23</v>
-      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -8237,9 +7623,6 @@
       <c r="I205" t="n">
         <v>0.01745025252485317</v>
       </c>
-      <c r="J205" t="n">
-        <v>349</v>
-      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -8277,9 +7660,6 @@
       <c r="I206" t="n">
         <v>0.008788713585665818</v>
       </c>
-      <c r="J206" t="n">
-        <v>175</v>
-      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -8317,9 +7697,6 @@
       <c r="I207" t="n">
         <v>0.001299024442283334</v>
       </c>
-      <c r="J207" t="n">
-        <v>25</v>
-      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -8357,9 +7734,6 @@
       <c r="I208" t="n">
         <v>0.009928547873711543</v>
       </c>
-      <c r="J208" t="n">
-        <v>198</v>
-      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -8397,9 +7771,6 @@
       <c r="I209" t="n">
         <v>0.009769322095030645</v>
       </c>
-      <c r="J209" t="n">
-        <v>195</v>
-      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -8437,9 +7808,6 @@
       <c r="I210" t="n">
         <v>0.0026129953235327</v>
       </c>
-      <c r="J210" t="n">
-        <v>52</v>
-      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -8477,9 +7845,6 @@
       <c r="I211" t="n">
         <v>0.007575918050534982</v>
       </c>
-      <c r="J211" t="n">
-        <v>151</v>
-      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -8517,9 +7882,6 @@
       <c r="I212" t="n">
         <v>0.01744980649412579</v>
       </c>
-      <c r="J212" t="n">
-        <v>348</v>
-      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -8557,9 +7919,6 @@
       <c r="I213" t="n">
         <v>0.007138235974947832</v>
       </c>
-      <c r="J213" t="n">
-        <v>142</v>
-      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -8597,9 +7956,6 @@
       <c r="I214" t="n">
         <v>0.002370264422552135</v>
       </c>
-      <c r="J214" t="n">
-        <v>47</v>
-      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -8637,9 +7993,6 @@
       <c r="I215" t="n">
         <v>0.002023090138162408</v>
       </c>
-      <c r="J215" t="n">
-        <v>40</v>
-      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -8677,9 +8030,6 @@
       <c r="I216" t="n">
         <v>0.001001163945964172</v>
       </c>
-      <c r="J216" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -8717,9 +8067,6 @@
       <c r="I217" t="n">
         <v>0.008926748106721035</v>
       </c>
-      <c r="J217" t="n">
-        <v>178</v>
-      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -8757,9 +8104,6 @@
       <c r="I218" t="n">
         <v>0.01389063325098344</v>
       </c>
-      <c r="J218" t="n">
-        <v>277</v>
-      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -8797,9 +8141,6 @@
       <c r="I219" t="n">
         <v>0.001305905490955689</v>
       </c>
-      <c r="J219" t="n">
-        <v>26</v>
-      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -8837,9 +8178,6 @@
       <c r="I220" t="n">
         <v>0.001419097496274391</v>
       </c>
-      <c r="J220" t="n">
-        <v>28</v>
-      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -8877,9 +8215,6 @@
       <c r="I221" t="n">
         <v>0.006011356962883819</v>
       </c>
-      <c r="J221" t="n">
-        <v>120</v>
-      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -8917,9 +8252,6 @@
       <c r="I222" t="n">
         <v>0.00457395811253391</v>
       </c>
-      <c r="J222" t="n">
-        <v>91</v>
-      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -8957,9 +8289,6 @@
       <c r="I223" t="n">
         <v>0.002016562651515491</v>
       </c>
-      <c r="J223" t="n">
-        <v>40</v>
-      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -8997,9 +8326,6 @@
       <c r="I224" t="n">
         <v>0.01155654217993961</v>
       </c>
-      <c r="J224" t="n">
-        <v>231</v>
-      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -9037,9 +8363,6 @@
       <c r="I225" t="n">
         <v>0.01151823995512512</v>
       </c>
-      <c r="J225" t="n">
-        <v>230</v>
-      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -9077,9 +8400,6 @@
       <c r="I226" t="n">
         <v>0.008580547946581177</v>
       </c>
-      <c r="J226" t="n">
-        <v>171</v>
-      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -9117,9 +8437,6 @@
       <c r="I227" t="n">
         <v>0.01273965775130613</v>
       </c>
-      <c r="J227" t="n">
-        <v>254</v>
-      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -9157,9 +8474,6 @@
       <c r="I228" t="n">
         <v>0.001981627011166354</v>
       </c>
-      <c r="J228" t="n">
-        <v>39</v>
-      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -9197,9 +8511,6 @@
       <c r="I229" t="n">
         <v>0.0009845639033975483</v>
       </c>
-      <c r="J229" t="n">
-        <v>19</v>
-      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -9237,9 +8548,6 @@
       <c r="I230" t="n">
         <v>0.001463387761790014</v>
       </c>
-      <c r="J230" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -9276,9 +8584,6 @@
       </c>
       <c r="I231" t="n">
         <v>0.01099307913534466</v>
-      </c>
-      <c r="J231" t="n">
-        <v>219</v>
       </c>
     </row>
     <row r="232">
@@ -9313,9 +8618,6 @@
       <c r="I232" t="n">
         <v>0.001885304453770596</v>
       </c>
-      <c r="J232" t="n">
-        <v>37</v>
-      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -9352,9 +8654,6 @@
       </c>
       <c r="I233" t="n">
         <v>0.002290121412409009</v>
-      </c>
-      <c r="J233" t="n">
-        <v>45</v>
       </c>
     </row>
     <row r="234">
@@ -9389,9 +8688,6 @@
       <c r="I234" t="n">
         <v>0.001896487222882698</v>
       </c>
-      <c r="J234" t="n">
-        <v>37</v>
-      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -9425,9 +8721,6 @@
       <c r="I235" t="n">
         <v>0.001516517103847819</v>
       </c>
-      <c r="J235" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -9461,9 +8754,6 @@
       <c r="I236" t="n">
         <v>0.005921872218046824</v>
       </c>
-      <c r="J236" t="n">
-        <v>118</v>
-      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -9500,9 +8790,6 @@
       </c>
       <c r="I237" t="n">
         <v>0.002335214321176321</v>
-      </c>
-      <c r="J237" t="n">
-        <v>46</v>
       </c>
     </row>
     <row r="238">
@@ -9537,9 +8824,6 @@
       <c r="I238" t="n">
         <v>0.001551399297134423</v>
       </c>
-      <c r="J238" t="n">
-        <v>31</v>
-      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -9577,9 +8861,6 @@
       <c r="I239" t="n">
         <v>0.005411233830410579</v>
       </c>
-      <c r="J239" t="n">
-        <v>108</v>
-      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -9617,9 +8898,6 @@
       <c r="I240" t="n">
         <v>0.004508899881724334</v>
       </c>
-      <c r="J240" t="n">
-        <v>90</v>
-      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -9657,9 +8935,6 @@
       <c r="I241" t="n">
         <v>0.01913672033879864</v>
       </c>
-      <c r="J241" t="n">
-        <v>382</v>
-      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -9697,9 +8972,6 @@
       <c r="I242" t="n">
         <v>0.008517315005657772</v>
       </c>
-      <c r="J242" t="n">
-        <v>170</v>
-      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -9737,9 +9009,6 @@
       <c r="I243" t="n">
         <v>0.007122090201228537</v>
       </c>
-      <c r="J243" t="n">
-        <v>142</v>
-      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -9777,9 +9046,6 @@
       <c r="I244" t="n">
         <v>0.004388577383613219</v>
       </c>
-      <c r="J244" t="n">
-        <v>87</v>
-      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -9816,9 +9082,6 @@
       </c>
       <c r="I245" t="n">
         <v>0.005365066005049762</v>
-      </c>
-      <c r="J245" t="n">
-        <v>107</v>
       </c>
     </row>
     <row r="246">
@@ -9853,9 +9116,6 @@
       <c r="I246" t="n">
         <v>0.009834590446140419</v>
       </c>
-      <c r="J246" t="n">
-        <v>196</v>
-      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -9893,9 +9153,6 @@
       <c r="I247" t="n">
         <v>0.004810915850683934</v>
       </c>
-      <c r="J247" t="n">
-        <v>96</v>
-      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -9933,9 +9190,6 @@
       <c r="I248" t="n">
         <v>0.007169250170868552</v>
       </c>
-      <c r="J248" t="n">
-        <v>143</v>
-      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -9973,9 +9227,6 @@
       <c r="I249" t="n">
         <v>0.001398910391213494</v>
       </c>
-      <c r="J249" t="n">
-        <v>27</v>
-      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -10013,9 +9264,6 @@
       <c r="I250" t="n">
         <v>0.007872666225730341</v>
       </c>
-      <c r="J250" t="n">
-        <v>157</v>
-      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -10053,9 +9301,6 @@
       <c r="I251" t="n">
         <v>0.004394699802897494</v>
       </c>
-      <c r="J251" t="n">
-        <v>87</v>
-      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -10093,9 +9338,6 @@
       <c r="I252" t="n">
         <v>0.004700238795335188</v>
       </c>
-      <c r="J252" t="n">
-        <v>94</v>
-      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -10133,9 +9375,6 @@
       <c r="I253" t="n">
         <v>0.005640547735439144</v>
       </c>
-      <c r="J253" t="n">
-        <v>112</v>
-      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -10173,9 +9412,6 @@
       <c r="I254" t="n">
         <v>0.003190323154800453</v>
       </c>
-      <c r="J254" t="n">
-        <v>63</v>
-      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -10213,9 +9449,6 @@
       <c r="I255" t="n">
         <v>0.002536740759003085</v>
       </c>
-      <c r="J255" t="n">
-        <v>50</v>
-      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -10253,9 +9486,6 @@
       <c r="I256" t="n">
         <v>0.001774167241208599</v>
       </c>
-      <c r="J256" t="n">
-        <v>35</v>
-      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -10293,9 +9523,6 @@
       <c r="I257" t="n">
         <v>0.002461907306194876</v>
       </c>
-      <c r="J257" t="n">
-        <v>49</v>
-      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -10333,9 +9560,6 @@
       <c r="I258" t="n">
         <v>0.001561390968852768</v>
       </c>
-      <c r="J258" t="n">
-        <v>31</v>
-      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -10373,9 +9597,6 @@
       <c r="I259" t="n">
         <v>0.005579315760718542</v>
       </c>
-      <c r="J259" t="n">
-        <v>111</v>
-      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -10413,9 +9634,6 @@
       <c r="I260" t="n">
         <v>0.001200001066062651</v>
       </c>
-      <c r="J260" t="n">
-        <v>24</v>
-      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -10453,9 +9671,6 @@
       <c r="I261" t="n">
         <v>0.004166216847913645</v>
       </c>
-      <c r="J261" t="n">
-        <v>83</v>
-      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -10493,9 +9708,6 @@
       <c r="I262" t="n">
         <v>0.01200679931202503</v>
       </c>
-      <c r="J262" t="n">
-        <v>240</v>
-      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -10533,9 +9745,6 @@
       <c r="I263" t="n">
         <v>0.002126528828571615</v>
       </c>
-      <c r="J263" t="n">
-        <v>42</v>
-      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -10573,9 +9782,6 @@
       <c r="I264" t="n">
         <v>0.002648285700343453</v>
       </c>
-      <c r="J264" t="n">
-        <v>52</v>
-      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -10613,9 +9819,6 @@
       <c r="I265" t="n">
         <v>0.004377050584932171</v>
       </c>
-      <c r="J265" t="n">
-        <v>87</v>
-      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -10653,9 +9856,6 @@
       <c r="I266" t="n">
         <v>0.002907242813976569</v>
       </c>
-      <c r="J266" t="n">
-        <v>58</v>
-      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -10693,9 +9893,6 @@
       <c r="I267" t="n">
         <v>0.002992159484048202</v>
       </c>
-      <c r="J267" t="n">
-        <v>59</v>
-      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -10733,9 +9930,6 @@
       <c r="I268" t="n">
         <v>0.002894892013908268</v>
       </c>
-      <c r="J268" t="n">
-        <v>57</v>
-      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -10773,9 +9967,6 @@
       <c r="I269" t="n">
         <v>0.001913927428603375</v>
       </c>
-      <c r="J269" t="n">
-        <v>38</v>
-      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -10813,9 +10004,6 @@
       <c r="I270" t="n">
         <v>0.002751458317967085</v>
       </c>
-      <c r="J270" t="n">
-        <v>55</v>
-      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -10853,9 +10041,6 @@
       <c r="I271" t="n">
         <v>0.001870423418143984</v>
       </c>
-      <c r="J271" t="n">
-        <v>37</v>
-      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -10893,9 +10078,6 @@
       <c r="I272" t="n">
         <v>0.002940316700170427</v>
       </c>
-      <c r="J272" t="n">
-        <v>58</v>
-      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -10933,9 +10115,6 @@
       <c r="I273" t="n">
         <v>0.008071148474858066</v>
       </c>
-      <c r="J273" t="n">
-        <v>161</v>
-      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -10973,9 +10152,6 @@
       <c r="I274" t="n">
         <v>0.004017674082798858</v>
       </c>
-      <c r="J274" t="n">
-        <v>80</v>
-      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -11013,9 +10189,6 @@
       <c r="I275" t="n">
         <v>0.007779743497041481</v>
       </c>
-      <c r="J275" t="n">
-        <v>155</v>
-      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -11053,9 +10226,6 @@
       <c r="I276" t="n">
         <v>0.004380672125320638</v>
       </c>
-      <c r="J276" t="n">
-        <v>87</v>
-      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -11093,9 +10263,6 @@
       <c r="I277" t="n">
         <v>0.004754093689893641</v>
       </c>
-      <c r="J277" t="n">
-        <v>95</v>
-      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -11133,9 +10300,6 @@
       <c r="I278" t="n">
         <v>0.004693154960105556</v>
       </c>
-      <c r="J278" t="n">
-        <v>93</v>
-      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -11173,9 +10337,6 @@
       <c r="I279" t="n">
         <v>0.009175557770535738</v>
       </c>
-      <c r="J279" t="n">
-        <v>183</v>
-      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -11213,9 +10374,6 @@
       <c r="I280" t="n">
         <v>0.02766931458254725</v>
       </c>
-      <c r="J280" t="n">
-        <v>553</v>
-      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -11253,9 +10411,6 @@
       <c r="I281" t="n">
         <v>0.001092840054905397</v>
       </c>
-      <c r="J281" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -11293,9 +10448,6 @@
       <c r="I282" t="n">
         <v>0.003724333573303042</v>
       </c>
-      <c r="J282" t="n">
-        <v>74</v>
-      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -11332,9 +10484,6 @@
       </c>
       <c r="I283" t="n">
         <v>0.003828574905337793</v>
-      </c>
-      <c r="J283" t="n">
-        <v>76</v>
       </c>
     </row>
     <row r="284">
@@ -11369,9 +10518,6 @@
       <c r="I284" t="n">
         <v>0.01139162111133482</v>
       </c>
-      <c r="J284" t="n">
-        <v>227</v>
-      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -11408,9 +10554,6 @@
       </c>
       <c r="I285" t="n">
         <v>0.01638018661054588</v>
-      </c>
-      <c r="J285" t="n">
-        <v>327</v>
       </c>
     </row>
     <row r="286">
@@ -11445,9 +10588,6 @@
       <c r="I286" t="n">
         <v>0.08729065452734033</v>
       </c>
-      <c r="J286" t="n">
-        <v>1745</v>
-      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -11481,9 +10621,6 @@
       <c r="I287" t="n">
         <v>0.08063626369491834</v>
       </c>
-      <c r="J287" t="n">
-        <v>1612</v>
-      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -11521,9 +10658,6 @@
       <c r="I288" t="n">
         <v>0.00191733747513724</v>
       </c>
-      <c r="J288" t="n">
-        <v>38</v>
-      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -11561,9 +10695,6 @@
       <c r="I289" t="n">
         <v>0.002258189679036713</v>
       </c>
-      <c r="J289" t="n">
-        <v>45</v>
-      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -11601,9 +10732,6 @@
       <c r="I290" t="n">
         <v>0.001677368384000519</v>
       </c>
-      <c r="J290" t="n">
-        <v>33</v>
-      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -11641,9 +10769,6 @@
       <c r="I291" t="n">
         <v>0.008801029398453369</v>
       </c>
-      <c r="J291" t="n">
-        <v>176</v>
-      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -11681,9 +10806,6 @@
       <c r="I292" t="n">
         <v>0.001674310973390568</v>
       </c>
-      <c r="J292" t="n">
-        <v>33</v>
-      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -11721,9 +10843,6 @@
       <c r="I293" t="n">
         <v>0.004890524935139002</v>
       </c>
-      <c r="J293" t="n">
-        <v>97</v>
-      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -11761,9 +10880,6 @@
       <c r="I294" t="n">
         <v>0.002193082809654799</v>
       </c>
-      <c r="J294" t="n">
-        <v>43</v>
-      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -11801,9 +10917,6 @@
       <c r="I295" t="n">
         <v>0.001877845295184839</v>
       </c>
-      <c r="J295" t="n">
-        <v>37</v>
-      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -11841,9 +10954,6 @@
       <c r="I296" t="n">
         <v>0.001765531115817079</v>
       </c>
-      <c r="J296" t="n">
-        <v>35</v>
-      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -11881,9 +10991,6 @@
       <c r="I297" t="n">
         <v>0.004114189427552733</v>
       </c>
-      <c r="J297" t="n">
-        <v>82</v>
-      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -11921,9 +11028,6 @@
       <c r="I298" t="n">
         <v>0.001623556362378627</v>
       </c>
-      <c r="J298" t="n">
-        <v>32</v>
-      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -11961,9 +11065,6 @@
       <c r="I299" t="n">
         <v>0.0027188346542313</v>
       </c>
-      <c r="J299" t="n">
-        <v>54</v>
-      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -12001,9 +11102,6 @@
       <c r="I300" t="n">
         <v>0.0027305020952502</v>
       </c>
-      <c r="J300" t="n">
-        <v>54</v>
-      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -12041,9 +11139,6 @@
       <c r="I301" t="n">
         <v>0.008143546430212827</v>
       </c>
-      <c r="J301" t="n">
-        <v>162</v>
-      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -12081,9 +11176,6 @@
       <c r="I302" t="n">
         <v>0.007825129182926887</v>
       </c>
-      <c r="J302" t="n">
-        <v>156</v>
-      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -12120,9 +11212,6 @@
       </c>
       <c r="I303" t="n">
         <v>0.01311857842867104</v>
-      </c>
-      <c r="J303" t="n">
-        <v>262</v>
       </c>
     </row>
     <row r="304">
@@ -12157,9 +11246,6 @@
       <c r="I304" t="n">
         <v>0.05611269784648801</v>
       </c>
-      <c r="J304" t="n">
-        <v>1122</v>
-      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -12197,9 +11283,6 @@
       <c r="I305" t="n">
         <v>0.008925431520896194</v>
       </c>
-      <c r="J305" t="n">
-        <v>178</v>
-      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -12237,9 +11320,6 @@
       <c r="I306" t="n">
         <v>0.003242265093308488</v>
       </c>
-      <c r="J306" t="n">
-        <v>64</v>
-      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -12277,9 +11357,6 @@
       <c r="I307" t="n">
         <v>0.002921074740983583</v>
       </c>
-      <c r="J307" t="n">
-        <v>58</v>
-      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -12317,9 +11394,6 @@
       <c r="I308" t="n">
         <v>0.002894640124453033</v>
       </c>
-      <c r="J308" t="n">
-        <v>57</v>
-      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -12357,9 +11431,6 @@
       <c r="I309" t="n">
         <v>0.0188763196798095</v>
       </c>
-      <c r="J309" t="n">
-        <v>377</v>
-      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -12397,9 +11468,6 @@
       <c r="I310" t="n">
         <v>0.009044808879372925</v>
       </c>
-      <c r="J310" t="n">
-        <v>180</v>
-      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -12437,9 +11505,6 @@
       <c r="I311" t="n">
         <v>0.00171051646470294</v>
       </c>
-      <c r="J311" t="n">
-        <v>34</v>
-      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -12476,9 +11541,6 @@
       </c>
       <c r="I312" t="n">
         <v>0.002732606856378181</v>
-      </c>
-      <c r="J312" t="n">
-        <v>54</v>
       </c>
     </row>
     <row r="313">
@@ -12513,9 +11575,6 @@
       <c r="I313" t="n">
         <v>0.002777792045732476</v>
       </c>
-      <c r="J313" t="n">
-        <v>55</v>
-      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -12549,9 +11608,6 @@
       <c r="I314" t="n">
         <v>0.01189681744759871</v>
       </c>
-      <c r="J314" t="n">
-        <v>237</v>
-      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -12589,9 +11645,6 @@
       <c r="I315" t="n">
         <v>0.01666439037684428</v>
       </c>
-      <c r="J315" t="n">
-        <v>333</v>
-      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -12628,9 +11681,6 @@
       </c>
       <c r="I316" t="n">
         <v>0.0102173017299941</v>
-      </c>
-      <c r="J316" t="n">
-        <v>204</v>
       </c>
     </row>
     <row r="317">
@@ -12665,9 +11715,6 @@
       <c r="I317" t="n">
         <v>0.007488334314004183</v>
       </c>
-      <c r="J317" t="n">
-        <v>149</v>
-      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -12705,9 +11752,6 @@
       <c r="I318" t="n">
         <v>0.002197449615716015</v>
       </c>
-      <c r="J318" t="n">
-        <v>43</v>
-      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -12745,9 +11789,6 @@
       <c r="I319" t="n">
         <v>0.001429989377336486</v>
       </c>
-      <c r="J319" t="n">
-        <v>28</v>
-      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -12785,9 +11826,6 @@
       <c r="I320" t="n">
         <v>0.01236596761254422</v>
       </c>
-      <c r="J320" t="n">
-        <v>247</v>
-      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -12824,9 +11862,6 @@
       </c>
       <c r="I321" t="n">
         <v>0.01233889082350791</v>
-      </c>
-      <c r="J321" t="n">
-        <v>246</v>
       </c>
     </row>
     <row r="322">
@@ -12861,9 +11896,6 @@
       <c r="I322" t="n">
         <v>0.01437021087356796</v>
       </c>
-      <c r="J322" t="n">
-        <v>287</v>
-      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -12897,9 +11929,6 @@
       <c r="I323" t="n">
         <v>0.007712069896840687</v>
       </c>
-      <c r="J323" t="n">
-        <v>154</v>
-      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -12937,9 +11966,6 @@
       <c r="I324" t="n">
         <v>0.004226701394703632</v>
       </c>
-      <c r="J324" t="n">
-        <v>84</v>
-      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -12976,9 +12002,6 @@
       </c>
       <c r="I325" t="n">
         <v>0.001465924905121968</v>
-      </c>
-      <c r="J325" t="n">
-        <v>29</v>
       </c>
     </row>
     <row r="326">
@@ -13013,9 +12036,6 @@
       <c r="I326" t="n">
         <v>0.0006844533906581482</v>
       </c>
-      <c r="J326" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -13049,9 +12069,6 @@
       <c r="I327" t="n">
         <v>0.108749980868844</v>
       </c>
-      <c r="J327" t="n">
-        <v>2174</v>
-      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -13089,9 +12106,6 @@
       <c r="I328" t="n">
         <v>0.000698916815660686</v>
       </c>
-      <c r="J328" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -13129,9 +12143,6 @@
       <c r="I329" t="n">
         <v>0.00880147829823456</v>
       </c>
-      <c r="J329" t="n">
-        <v>176</v>
-      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -13169,9 +12180,6 @@
       <c r="I330" t="n">
         <v>0.0006789186056292125</v>
       </c>
-      <c r="J330" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -13209,9 +12217,6 @@
       <c r="I331" t="n">
         <v>0.0005734296052410973</v>
       </c>
-      <c r="J331" t="n">
-        <v>11</v>
-      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -13249,9 +12254,6 @@
       <c r="I332" t="n">
         <v>0.009382831804963302</v>
       </c>
-      <c r="J332" t="n">
-        <v>187</v>
-      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -13289,9 +12291,6 @@
       <c r="I333" t="n">
         <v>0.0009985544587692509</v>
       </c>
-      <c r="J333" t="n">
-        <v>19</v>
-      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -13329,9 +12328,6 @@
       <c r="I334" t="n">
         <v>0.001200876170996057</v>
       </c>
-      <c r="J334" t="n">
-        <v>24</v>
-      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -13369,9 +12365,6 @@
       <c r="I335" t="n">
         <v>0.000530220242952823</v>
       </c>
-      <c r="J335" t="n">
-        <v>10</v>
-      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -13409,9 +12402,6 @@
       <c r="I336" t="n">
         <v>0.01041603989787185</v>
       </c>
-      <c r="J336" t="n">
-        <v>208</v>
-      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -13448,9 +12438,6 @@
       </c>
       <c r="I337" t="n">
         <v>0.01219696291845105</v>
-      </c>
-      <c r="J337" t="n">
-        <v>243</v>
       </c>
     </row>
     <row r="338">
@@ -13485,9 +12472,6 @@
       <c r="I338" t="n">
         <v>0.0101774159709819</v>
       </c>
-      <c r="J338" t="n">
-        <v>203</v>
-      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -13525,9 +12509,6 @@
       <c r="I339" t="n">
         <v>0.001536233204887122</v>
       </c>
-      <c r="J339" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -13565,9 +12546,6 @@
       <c r="I340" t="n">
         <v>0.0002413814798690334</v>
       </c>
-      <c r="J340" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -13605,9 +12583,6 @@
       <c r="I341" t="n">
         <v>0.009395168471715894</v>
       </c>
-      <c r="J341" t="n">
-        <v>187</v>
-      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -13644,9 +12619,6 @@
       </c>
       <c r="I342" t="n">
         <v>0.007408653206845429</v>
-      </c>
-      <c r="J342" t="n">
-        <v>148</v>
       </c>
     </row>
     <row r="343">
@@ -13681,9 +12653,6 @@
       <c r="I343" t="n">
         <v>0.03046974043181306</v>
       </c>
-      <c r="J343" t="n">
-        <v>609</v>
-      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -13717,9 +12686,6 @@
       <c r="I344" t="n">
         <v>0.001399571321960459</v>
       </c>
-      <c r="J344" t="n">
-        <v>27</v>
-      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -13753,9 +12719,6 @@
       <c r="I345" t="n">
         <v>0.004730906466264987</v>
       </c>
-      <c r="J345" t="n">
-        <v>94</v>
-      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -13789,9 +12752,6 @@
       <c r="I346" t="n">
         <v>0.02978378199554574</v>
       </c>
-      <c r="J346" t="n">
-        <v>595</v>
-      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -13825,9 +12785,6 @@
       <c r="I347" t="n">
         <v>0.002044755957524446</v>
       </c>
-      <c r="J347" t="n">
-        <v>40</v>
-      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -13864,9 +12821,6 @@
       </c>
       <c r="I348" t="n">
         <v>0.002055941174592837</v>
-      </c>
-      <c r="J348" t="n">
-        <v>41</v>
       </c>
     </row>
     <row r="349">
@@ -13901,9 +12855,6 @@
       <c r="I349" t="n">
         <v>0.03808959509384154</v>
       </c>
-      <c r="J349" t="n">
-        <v>761</v>
-      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -13937,9 +12888,6 @@
       <c r="I350" t="n">
         <v>0.002044581484525885</v>
       </c>
-      <c r="J350" t="n">
-        <v>40</v>
-      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -13976,9 +12924,6 @@
       </c>
       <c r="I351" t="n">
         <v>0.002058574484884397</v>
-      </c>
-      <c r="J351" t="n">
-        <v>41</v>
       </c>
     </row>
     <row r="352">
@@ -14013,9 +12958,6 @@
       <c r="I352" t="n">
         <v>0.09728630788275433</v>
       </c>
-      <c r="J352" t="n">
-        <v>1945</v>
-      </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -14049,9 +12991,6 @@
       <c r="I353" t="n">
         <v>0.03720404508318627</v>
       </c>
-      <c r="J353" t="n">
-        <v>744</v>
-      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -14085,9 +13024,6 @@
       <c r="I354" t="n">
         <v>0.00933535474195623</v>
       </c>
-      <c r="J354" t="n">
-        <v>186</v>
-      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -14121,9 +13057,6 @@
       <c r="I355" t="n">
         <v>0.009184906566476598</v>
       </c>
-      <c r="J355" t="n">
-        <v>183</v>
-      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -14157,9 +13090,6 @@
       <c r="I356" t="n">
         <v>0.08262526559536514</v>
       </c>
-      <c r="J356" t="n">
-        <v>1652</v>
-      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -14193,9 +13123,6 @@
       <c r="I357" t="n">
         <v>0.002698331333824327</v>
       </c>
-      <c r="J357" t="n">
-        <v>53</v>
-      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -14229,9 +13156,6 @@
       <c r="I358" t="n">
         <v>0.002724001854300357</v>
       </c>
-      <c r="J358" t="n">
-        <v>54</v>
-      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -14269,9 +13193,6 @@
       <c r="I359" t="n">
         <v>0.01663459428711831</v>
       </c>
-      <c r="J359" t="n">
-        <v>332</v>
-      </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -14308,9 +13229,6 @@
       </c>
       <c r="I360" t="n">
         <v>0.01490900366902023</v>
-      </c>
-      <c r="J360" t="n">
-        <v>298</v>
       </c>
     </row>
     <row r="361">
@@ -14345,9 +13263,6 @@
       <c r="I361" t="n">
         <v>0.03999520984231772</v>
       </c>
-      <c r="J361" t="n">
-        <v>799</v>
-      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -14381,9 +13296,6 @@
       <c r="I362" t="n">
         <v>0.09749866892750156</v>
       </c>
-      <c r="J362" t="n">
-        <v>1949</v>
-      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -14417,9 +13329,6 @@
       <c r="I363" t="n">
         <v>0.1029255749343955</v>
       </c>
-      <c r="J363" t="n">
-        <v>2058</v>
-      </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -14453,9 +13362,6 @@
       <c r="I364" t="n">
         <v>0.002845274109218796</v>
       </c>
-      <c r="J364" t="n">
-        <v>56</v>
-      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -14489,9 +13395,6 @@
       <c r="I365" t="n">
         <v>0.002844559560407342</v>
       </c>
-      <c r="J365" t="n">
-        <v>56</v>
-      </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -14525,9 +13428,6 @@
       <c r="I366" t="n">
         <v>0.001386584321538204</v>
       </c>
-      <c r="J366" t="n">
-        <v>27</v>
-      </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -14561,9 +13461,6 @@
       <c r="I367" t="n">
         <v>0.001460962514465192</v>
       </c>
-      <c r="J367" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -14597,9 +13494,6 @@
       <c r="I368" t="n">
         <v>0.001493429156641299</v>
       </c>
-      <c r="J368" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -14633,9 +13527,6 @@
       <c r="I369" t="n">
         <v>0.001420047445985149</v>
       </c>
-      <c r="J369" t="n">
-        <v>28</v>
-      </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -14669,9 +13560,6 @@
       <c r="I370" t="n">
         <v>0.001800014865564987</v>
       </c>
-      <c r="J370" t="n">
-        <v>36</v>
-      </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -14705,9 +13593,6 @@
       <c r="I371" t="n">
         <v>0.001799465317123119</v>
       </c>
-      <c r="J371" t="n">
-        <v>35</v>
-      </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -14741,9 +13626,6 @@
       <c r="I372" t="n">
         <v>0.1024750467751829</v>
       </c>
-      <c r="J372" t="n">
-        <v>2049</v>
-      </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -14777,9 +13659,6 @@
       <c r="I373" t="n">
         <v>0.0009056626344670699</v>
       </c>
-      <c r="J373" t="n">
-        <v>18</v>
-      </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -14813,9 +13692,6 @@
       <c r="I374" t="n">
         <v>0.0009053719186137897</v>
       </c>
-      <c r="J374" t="n">
-        <v>18</v>
-      </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -14849,9 +13725,6 @@
       <c r="I375" t="n">
         <v>0.0009052156883688769</v>
       </c>
-      <c r="J375" t="n">
-        <v>18</v>
-      </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -14885,9 +13758,6 @@
       <c r="I376" t="n">
         <v>0.0009053870958059091</v>
       </c>
-      <c r="J376" t="n">
-        <v>18</v>
-      </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -14924,9 +13794,6 @@
       </c>
       <c r="I377" t="n">
         <v>0.01566155178758649</v>
-      </c>
-      <c r="J377" t="n">
-        <v>313</v>
       </c>
     </row>
     <row r="378">
@@ -14961,9 +13828,6 @@
       <c r="I378" t="n">
         <v>0.001811701112940273</v>
       </c>
-      <c r="J378" t="n">
-        <v>36</v>
-      </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -15001,9 +13865,6 @@
       <c r="I379" t="n">
         <v>0.02367684304253539</v>
       </c>
-      <c r="J379" t="n">
-        <v>473</v>
-      </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -15041,9 +13902,6 @@
       <c r="I380" t="n">
         <v>0.001635237339683526</v>
       </c>
-      <c r="J380" t="n">
-        <v>32</v>
-      </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -15081,9 +13939,6 @@
       <c r="I381" t="n">
         <v>0.001122131021297757</v>
       </c>
-      <c r="J381" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -15121,9 +13976,6 @@
       <c r="I382" t="n">
         <v>0.001267513596538635</v>
       </c>
-      <c r="J382" t="n">
-        <v>25</v>
-      </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -15161,9 +14013,6 @@
       <c r="I383" t="n">
         <v>0.001204989969319641</v>
       </c>
-      <c r="J383" t="n">
-        <v>24</v>
-      </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -15201,9 +14050,6 @@
       <c r="I384" t="n">
         <v>0.008989869217608625</v>
       </c>
-      <c r="J384" t="n">
-        <v>179</v>
-      </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
@@ -15241,9 +14087,6 @@
       <c r="I385" t="n">
         <v>0.003973627704397627</v>
       </c>
-      <c r="J385" t="n">
-        <v>79</v>
-      </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -15281,9 +14124,6 @@
       <c r="I386" t="n">
         <v>0.01220279270305961</v>
       </c>
-      <c r="J386" t="n">
-        <v>244</v>
-      </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
@@ -15320,9 +14160,6 @@
       </c>
       <c r="I387" t="n">
         <v>0.004978242373651362</v>
-      </c>
-      <c r="J387" t="n">
-        <v>99</v>
       </c>
     </row>
     <row r="388">
@@ -15357,9 +14194,6 @@
       <c r="I388" t="n">
         <v>0.002023498866013619</v>
       </c>
-      <c r="J388" t="n">
-        <v>40</v>
-      </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
@@ -15393,9 +14227,6 @@
       <c r="I389" t="n">
         <v>0.001740587918210426</v>
       </c>
-      <c r="J389" t="n">
-        <v>34</v>
-      </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
@@ -15429,9 +14260,6 @@
       <c r="I390" t="n">
         <v>0.01743339520289647</v>
       </c>
-      <c r="J390" t="n">
-        <v>348</v>
-      </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
@@ -15465,9 +14293,6 @@
       <c r="I391" t="n">
         <v>0.0175233934215727</v>
       </c>
-      <c r="J391" t="n">
-        <v>350</v>
-      </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
@@ -15501,9 +14326,6 @@
       <c r="I392" t="n">
         <v>0.01535396266370047</v>
       </c>
-      <c r="J392" t="n">
-        <v>307</v>
-      </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
@@ -15536,9 +14358,6 @@
       </c>
       <c r="I393" t="n">
         <v>0.02999602493895049</v>
-      </c>
-      <c r="J393" t="n">
-        <v>599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>